<commit_message>
Added animation and Player state controller.
Added animation for walk, jump and attack. As well as a state controller for the player to manage it's states and animations.
</commit_message>
<xml_diff>
--- a/ElemntalsFight_Asset_Inventory.xlsx
+++ b/ElemntalsFight_Asset_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\GitHub\Elementals-Fight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CF64D4-98A6-4AC6-A09F-23E109D84193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F213D753-4688-4DB6-88EC-C0FCFB5043E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{01B14A2B-A28C-7B4F-8941-09249883C81A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Asset Group</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>https://assetstore.unity.com/packages/2d/textures-materials/floors/yughues-free-ground-materials-13001</t>
+  </si>
+  <si>
+    <t>Animations</t>
+  </si>
+  <si>
+    <t>MageAnimations</t>
+  </si>
+  <si>
+    <t>Frank_Mage</t>
+  </si>
+  <si>
+    <t>Animation clips in Mage animation folder are copied from here due to import errors</t>
   </si>
 </sst>
 </file>
@@ -623,7 +635,7 @@
   <dimension ref="A2:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -712,7 +724,18 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7"/>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>